<commit_message>
Sprememba v bilanci, IPI in IDT za podjetje pumo
</commit_message>
<xml_diff>
--- a/Data-Nike/Bilanca_nike.xlsx
+++ b/Data-Nike/Bilanca_nike.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marko\Documents\AMAT\Analiza-podjetij\Data-Nike\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristina\Desktop\Študijsko leto 2020-21\TFPR\Analiza-podjetij\Data-Nike\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Assets</t>
   </si>
@@ -124,7 +124,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="###,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +154,21 @@
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="3">
@@ -211,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -236,6 +251,21 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -518,18 +548,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="14.7109375" customWidth="1"/>
+    <col min="1" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>43616</v>
@@ -543,8 +573,11 @@
       <c r="E1" s="2">
         <v>42521</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="10">
+        <v>42155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -552,8 +585,9 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -569,8 +603,11 @@
       <c r="E3" s="5">
         <v>6354000</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F3" s="11">
+        <v>6010000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -586,8 +623,11 @@
       <c r="E4" s="5">
         <v>412000</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F4" s="11">
+        <v>412000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -603,8 +643,11 @@
       <c r="E5" s="5">
         <v>3520000</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F5" s="11">
+        <v>3011000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -620,8 +663,11 @@
       <c r="E6" s="5">
         <v>2422000</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="11">
+        <v>2587000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -637,8 +683,11 @@
       <c r="E7" s="5">
         <v>15025000</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="11">
+        <v>15587000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -654,8 +703,11 @@
       <c r="E8" s="5">
         <v>4838000</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="11">
+        <v>4337000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -671,8 +723,11 @@
       <c r="E9" s="5">
         <v>3241000</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F9" s="11">
+        <v>3358000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -688,8 +743,11 @@
       <c r="E10" s="5">
         <v>6946000</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F10" s="11">
+        <v>7892000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -705,8 +763,11 @@
       <c r="E11" s="5">
         <v>5457000</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="11">
+        <v>5924000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -722,8 +783,11 @@
       <c r="E12" s="7">
         <v>21379000</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F12" s="12">
+        <v>21597000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -731,8 +795,9 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -748,8 +813,11 @@
       <c r="E14" s="5">
         <v>12258000</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="11">
+        <v>12707000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -765,8 +833,11 @@
       <c r="E15" s="5">
         <v>3000</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="F15" s="11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
@@ -782,8 +853,11 @@
       <c r="E16" s="5">
         <v>12255000</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F16" s="11">
+        <v>12704000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -799,8 +873,11 @@
       <c r="E17" s="5">
         <v>3763000</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F17" s="11">
+        <v>2558000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -816,8 +893,11 @@
       <c r="E18" s="5">
         <v>1993000</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F18" s="11">
+        <v>1079000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -833,8 +913,11 @@
       <c r="E19" s="5">
         <v>1770000</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="11">
+        <v>1479000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -850,8 +933,11 @@
       <c r="E20" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F20" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -867,8 +953,11 @@
       <c r="E21" s="5">
         <v>5358000</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="11">
+        <v>6332000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -884,8 +973,11 @@
       <c r="E22" s="5">
         <v>44000</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="11">
+        <v>107000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
@@ -901,8 +993,11 @@
       <c r="E23" s="5">
         <v>2191000</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F23" s="11">
+        <v>2131000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
@@ -918,8 +1013,11 @@
       <c r="E24" s="5">
         <v>3123000</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F24" s="11">
+        <v>4094000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>24</v>
       </c>
@@ -935,8 +1033,11 @@
       <c r="E25" s="7">
         <v>21379000</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="12">
+        <v>21597000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -944,8 +1045,9 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
@@ -961,8 +1063,11 @@
       <c r="E27" s="5">
         <v>5888000</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F27" s="11">
+        <v>5564000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>27</v>
       </c>
@@ -978,8 +1083,11 @@
       <c r="E28" s="9">
         <v>9667000</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F28" s="14">
+        <v>9255000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
@@ -995,8 +1103,11 @@
       <c r="E29" s="9">
         <v>70104775.964069605</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F29" s="14">
+        <v>64694223.414803401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
@@ -1012,8 +1123,12 @@
       <c r="E30" s="9">
         <v>70700</v>
       </c>
+      <c r="F30" s="14">
+        <v>62600</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>